<commit_message>
Edits to HTML Sample
</commit_message>
<xml_diff>
--- a/Sample Forms/HTML Formatting/HTMLFormatting.xlsx
+++ b/Sample Forms/HTML Formatting/HTMLFormatting.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hann7066\ArcGIS\My Survey Designs\HTMLFormatting 1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="156" yWindow="0" windowWidth="18756" windowHeight="12276" tabRatio="272"/>
   </bookViews>
@@ -657,9 +662,6 @@
     <t>Italics</t>
   </si>
   <si>
-    <t>&lt;i&gt;This text is italllized or however you spell it&lt;/i&gt;</t>
-  </si>
-  <si>
     <t>H1</t>
   </si>
   <si>
@@ -690,18 +692,6 @@
     <t>One word is &lt;u&gt;underlined&lt;/u&gt;</t>
   </si>
   <si>
-    <t>sub</t>
-  </si>
-  <si>
-    <t>One word is &lt;tt&gt;typewrite font&lt;/tt&gt;</t>
-  </si>
-  <si>
-    <t>One word is &lt;s&gt;typewrite font&lt;/s&gt;</t>
-  </si>
-  <si>
-    <t>lists</t>
-  </si>
-  <si>
     <t>Typewrite</t>
   </si>
   <si>
@@ -720,10 +710,25 @@
     <t>FONT2</t>
   </si>
   <si>
-    <t>euro</t>
-  </si>
-  <si>
     <t>&lt;p&gt;I will display &amp;euro;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>One word is &lt;tt&gt;typewrite&lt;/tt&gt; font</t>
+  </si>
+  <si>
+    <t>One word is &lt;s&gt;strikethrough&lt;/s&gt; font</t>
+  </si>
+  <si>
+    <t>Strikethrough</t>
+  </si>
+  <si>
+    <t>Lists</t>
+  </si>
+  <si>
+    <t>Euro</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;This text is in italics&lt;/i&gt;</t>
   </si>
 </sst>
 </file>
@@ -889,22 +894,6 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -936,6 +925,22 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1038,15 +1043,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:P234" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:P234" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:P234"/>
   <tableColumns count="16">
     <tableColumn id="1" name="type"/>
     <tableColumn id="2" name="name"/>
-    <tableColumn id="3" name="label" dataDxfId="4"/>
-    <tableColumn id="4" name="hint" dataDxfId="3"/>
+    <tableColumn id="3" name="label" dataDxfId="2"/>
+    <tableColumn id="4" name="hint" dataDxfId="1"/>
     <tableColumn id="5" name="constraint"/>
-    <tableColumn id="6" name="constraint_message" dataDxfId="2"/>
+    <tableColumn id="6" name="constraint_message" dataDxfId="0"/>
     <tableColumn id="7" name="required"/>
     <tableColumn id="8" name="appearance"/>
     <tableColumn id="9" name="default"/>
@@ -1436,9 +1441,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C18" sqref="C18"/>
+      <selection pane="topRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.33203125" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1558,7 +1563,7 @@
         <v>209</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -1567,10 +1572,10 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -1579,10 +1584,10 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1590,10 +1595,10 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1601,10 +1606,10 @@
         <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1612,10 +1617,10 @@
         <v>29</v>
       </c>
       <c r="B10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1623,10 +1628,10 @@
         <v>29</v>
       </c>
       <c r="B11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1634,10 +1639,10 @@
         <v>29</v>
       </c>
       <c r="B12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1645,10 +1650,10 @@
         <v>29</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1656,10 +1661,10 @@
         <v>29</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1667,10 +1672,10 @@
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1681,16 +1686,16 @@
         <v>231</v>
       </c>
       <c r="C16" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B12 B15:B231">
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <dataValidations count="12">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Label" prompt="The label will act as the question in your survey (e.g., What is your name?)." sqref="C1:C2 C4:C15 C17:C1048576"/>

</xml_diff>